<commit_message>
Tape4Backup LTO7 URLs updated to the correct product page.
</commit_message>
<xml_diff>
--- a/Internet_Pricing_All_2022-08-11.xlsx
+++ b/Internet_Pricing_All_2022-08-11.xlsx
@@ -458,16 +458,16 @@
         <v>5</v>
       </c>
       <c r="B4" s="1">
-        <v>41.6</v>
+        <v>42.95</v>
       </c>
       <c r="C4" s="1">
-        <v>40.15</v>
+        <v>42.5</v>
       </c>
       <c r="D4" s="1">
-        <v>40.15</v>
+        <v>42.15</v>
       </c>
       <c r="E4" s="1">
-        <v>41.15</v>
+        <v>44.75</v>
       </c>
     </row>
     <row r="5" spans="1:5">

</xml_diff>